<commit_message>
Inclusion of Optimal Power Flow
</commit_message>
<xml_diff>
--- a/Input Data - Resources 1.xlsx
+++ b/Input Data - Resources 1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hugo.serrano\PycharmProjects1\CRETE_VALLEY_T.4.3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1756455-D92F-4386-BDD0-A1E0EF9BAFED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDE619BC-2635-4EB3-A886-B0FD24037D39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="907" activeTab="3" xr2:uid="{A643D732-D500-40EC-92C3-BB1380872BE9}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="907" activeTab="3" xr2:uid="{A643D732-D500-40EC-92C3-BB1380872BE9}"/>
   </bookViews>
   <sheets>
     <sheet name="Electrical load" sheetId="1" r:id="rId1"/>
@@ -589,6 +589,15 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -605,15 +614,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -932,8 +932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{293146E6-8E2D-4ADC-82E7-CE7DA50FFBD7}">
   <dimension ref="A2:Z43"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W27" sqref="W27"/>
+    <sheetView showGridLines="0" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18:Z18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1180,76 +1180,76 @@
         <v>3</v>
       </c>
       <c r="C5" s="54">
-        <v>5</v>
+        <v>25.347000000000001</v>
       </c>
       <c r="D5" s="54">
-        <v>6</v>
+        <v>25.552</v>
       </c>
       <c r="E5" s="54">
-        <v>5</v>
+        <v>24.72</v>
       </c>
       <c r="F5" s="54">
-        <v>6</v>
+        <v>24.783999999999999</v>
       </c>
       <c r="G5" s="54">
-        <v>6</v>
+        <v>25.861999999999998</v>
       </c>
       <c r="H5" s="54">
-        <v>6</v>
+        <v>25.306000000000001</v>
       </c>
       <c r="I5" s="54">
-        <v>9.6000000000000014</v>
+        <v>40.2592</v>
       </c>
       <c r="J5" s="54">
-        <v>11</v>
+        <v>33.139000000000003</v>
       </c>
       <c r="K5" s="54">
-        <v>23</v>
+        <v>36.621000000000002</v>
       </c>
       <c r="L5" s="54">
-        <v>25</v>
+        <v>44.304000000000002</v>
       </c>
       <c r="M5" s="54">
-        <v>24</v>
+        <v>53.628999999999998</v>
       </c>
       <c r="N5" s="54">
-        <v>25</v>
+        <v>57.616999999999997</v>
       </c>
       <c r="O5" s="54">
-        <v>27</v>
+        <v>55.176000000000002</v>
       </c>
       <c r="P5" s="54">
-        <v>23</v>
+        <v>58.177</v>
       </c>
       <c r="Q5" s="54">
-        <v>21</v>
+        <v>58.219000000000001</v>
       </c>
       <c r="R5" s="54">
-        <v>21</v>
+        <v>54.584000000000003</v>
       </c>
       <c r="S5" s="54">
-        <v>17</v>
+        <v>51.578000000000003</v>
       </c>
       <c r="T5" s="54">
-        <v>34.5</v>
+        <v>65.9178</v>
       </c>
       <c r="U5" s="54">
-        <v>30</v>
+        <v>63.375999999999998</v>
       </c>
       <c r="V5" s="54">
-        <v>31</v>
+        <v>69.558000000000007</v>
       </c>
       <c r="W5" s="54">
-        <v>28</v>
+        <v>68.349000000000004</v>
       </c>
       <c r="X5" s="54">
-        <v>7</v>
+        <v>26.768000000000001</v>
       </c>
       <c r="Y5" s="54">
-        <v>6</v>
+        <v>26.358000000000001</v>
       </c>
       <c r="Z5" s="54">
-        <v>5</v>
+        <v>25.446000000000002</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.35">
@@ -1719,76 +1719,76 @@
         <v>10</v>
       </c>
       <c r="C12" s="54">
-        <v>0</v>
+        <v>25.347000000000001</v>
       </c>
       <c r="D12" s="54">
-        <v>0</v>
+        <v>25.552</v>
       </c>
       <c r="E12" s="54">
-        <v>0</v>
+        <v>24.72</v>
       </c>
       <c r="F12" s="54">
-        <v>0</v>
+        <v>24.783999999999999</v>
       </c>
       <c r="G12" s="54">
-        <v>0</v>
+        <v>25.861999999999998</v>
       </c>
       <c r="H12" s="54">
-        <v>0</v>
+        <v>25.306000000000001</v>
       </c>
       <c r="I12" s="54">
-        <v>0</v>
+        <v>40.2592</v>
       </c>
       <c r="J12" s="54">
-        <v>0</v>
+        <v>33.139000000000003</v>
       </c>
       <c r="K12" s="54">
-        <v>0</v>
+        <v>36.621000000000002</v>
       </c>
       <c r="L12" s="54">
-        <v>0</v>
+        <v>44.304000000000002</v>
       </c>
       <c r="M12" s="54">
-        <v>0</v>
+        <v>53.628999999999998</v>
       </c>
       <c r="N12" s="54">
-        <v>0</v>
+        <v>57.616999999999997</v>
       </c>
       <c r="O12" s="54">
-        <v>0</v>
+        <v>55.176000000000002</v>
       </c>
       <c r="P12" s="54">
-        <v>0</v>
+        <v>58.177</v>
       </c>
       <c r="Q12" s="54">
-        <v>0</v>
+        <v>58.219000000000001</v>
       </c>
       <c r="R12" s="54">
-        <v>0</v>
+        <v>54.584000000000003</v>
       </c>
       <c r="S12" s="54">
-        <v>0</v>
+        <v>51.578000000000003</v>
       </c>
       <c r="T12" s="54">
-        <v>0</v>
+        <v>65.9178</v>
       </c>
       <c r="U12" s="54">
-        <v>0</v>
+        <v>63.375999999999998</v>
       </c>
       <c r="V12" s="54">
-        <v>0</v>
+        <v>69.558000000000007</v>
       </c>
       <c r="W12" s="54">
-        <v>0</v>
+        <v>68.349000000000004</v>
       </c>
       <c r="X12" s="54">
-        <v>0</v>
+        <v>26.768000000000001</v>
       </c>
       <c r="Y12" s="54">
-        <v>0</v>
+        <v>26.358000000000001</v>
       </c>
       <c r="Z12" s="54">
-        <v>0</v>
+        <v>25.446000000000002</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.35">
@@ -2181,76 +2181,76 @@
         <v>16</v>
       </c>
       <c r="C18" s="54">
-        <v>98</v>
+        <v>77.081639600000003</v>
       </c>
       <c r="D18" s="54">
-        <v>92</v>
+        <v>76.205639599999998</v>
       </c>
       <c r="E18" s="54">
-        <v>90</v>
+        <v>77.573806099999999</v>
       </c>
       <c r="F18" s="54">
-        <v>91</v>
+        <v>75.894639600000005</v>
       </c>
       <c r="G18" s="54">
-        <v>90</v>
+        <v>76.521139499999904</v>
       </c>
       <c r="H18" s="54">
-        <v>97</v>
+        <v>78.041639599999996</v>
       </c>
       <c r="I18" s="54">
-        <v>254.4</v>
+        <v>138.90155632000003</v>
       </c>
       <c r="J18" s="54">
-        <v>206</v>
+        <v>107.0398029</v>
       </c>
       <c r="K18" s="54">
-        <v>240</v>
+        <v>141.36430200000001</v>
       </c>
       <c r="L18" s="54">
-        <v>291</v>
+        <v>174.7566344</v>
       </c>
       <c r="M18" s="54">
-        <v>318</v>
+        <v>176.8601353</v>
       </c>
       <c r="N18" s="54">
-        <v>323</v>
+        <v>176.50713210000001</v>
       </c>
       <c r="O18" s="54">
-        <v>322</v>
+        <v>176.68196620000001</v>
       </c>
       <c r="P18" s="54">
-        <v>308</v>
+        <v>177.60013069999999</v>
       </c>
       <c r="Q18" s="54">
-        <v>303</v>
+        <v>173.07829939999999</v>
       </c>
       <c r="R18" s="54">
-        <v>299</v>
+        <v>172.9864657</v>
       </c>
       <c r="S18" s="54">
-        <v>289</v>
+        <v>171.86096659999899</v>
       </c>
       <c r="T18" s="54">
-        <v>408</v>
+        <v>254.45574360000003</v>
       </c>
       <c r="U18" s="54">
-        <v>436</v>
+        <v>213.27413530000001</v>
       </c>
       <c r="V18" s="54">
-        <v>429</v>
+        <v>201.42347029999999</v>
       </c>
       <c r="W18" s="54">
-        <v>395</v>
+        <v>193.4893036</v>
       </c>
       <c r="X18" s="54">
-        <v>191</v>
+        <v>90.646970199999998</v>
       </c>
       <c r="Y18" s="54">
-        <v>186</v>
+        <v>86.497136900000001</v>
       </c>
       <c r="Z18" s="54">
-        <v>179</v>
+        <v>84.372804500000001</v>
       </c>
     </row>
     <row r="19" spans="2:26" x14ac:dyDescent="0.35">
@@ -2258,76 +2258,76 @@
         <v>17</v>
       </c>
       <c r="C19" s="54">
-        <v>0</v>
+        <v>77.081639600000003</v>
       </c>
       <c r="D19" s="54">
-        <v>0</v>
+        <v>76.205639599999998</v>
       </c>
       <c r="E19" s="54">
-        <v>0</v>
+        <v>77.573806099999999</v>
       </c>
       <c r="F19" s="54">
-        <v>0</v>
+        <v>75.894639600000005</v>
       </c>
       <c r="G19" s="54">
-        <v>0</v>
+        <v>76.521139499999904</v>
       </c>
       <c r="H19" s="54">
-        <v>0</v>
+        <v>78.041639599999996</v>
       </c>
       <c r="I19" s="54">
-        <v>0</v>
+        <v>138.90155632000003</v>
       </c>
       <c r="J19" s="54">
-        <v>0</v>
+        <v>107.0398029</v>
       </c>
       <c r="K19" s="54">
-        <v>0</v>
+        <v>141.36430200000001</v>
       </c>
       <c r="L19" s="54">
-        <v>0</v>
+        <v>174.7566344</v>
       </c>
       <c r="M19" s="54">
-        <v>0</v>
+        <v>176.8601353</v>
       </c>
       <c r="N19" s="54">
-        <v>0</v>
+        <v>176.50713210000001</v>
       </c>
       <c r="O19" s="54">
-        <v>0</v>
+        <v>176.68196620000001</v>
       </c>
       <c r="P19" s="54">
-        <v>0</v>
+        <v>177.60013069999999</v>
       </c>
       <c r="Q19" s="54">
-        <v>0</v>
+        <v>173.07829939999999</v>
       </c>
       <c r="R19" s="54">
-        <v>0</v>
+        <v>172.9864657</v>
       </c>
       <c r="S19" s="54">
-        <v>0</v>
+        <v>171.86096659999899</v>
       </c>
       <c r="T19" s="54">
-        <v>0</v>
+        <v>254.45574360000003</v>
       </c>
       <c r="U19" s="54">
-        <v>0</v>
+        <v>213.27413530000001</v>
       </c>
       <c r="V19" s="54">
-        <v>0</v>
+        <v>201.42347029999999</v>
       </c>
       <c r="W19" s="54">
-        <v>0</v>
+        <v>193.4893036</v>
       </c>
       <c r="X19" s="54">
-        <v>0</v>
+        <v>90.646970199999998</v>
       </c>
       <c r="Y19" s="54">
-        <v>0</v>
+        <v>86.497136900000001</v>
       </c>
       <c r="Z19" s="54">
-        <v>0</v>
+        <v>84.372804500000001</v>
       </c>
     </row>
     <row r="20" spans="2:26" x14ac:dyDescent="0.35">
@@ -2566,76 +2566,76 @@
         <v>21</v>
       </c>
       <c r="C23" s="54">
-        <v>0</v>
+        <v>506.14800000000002</v>
       </c>
       <c r="D23" s="54">
-        <v>0</v>
+        <v>494.697</v>
       </c>
       <c r="E23" s="54">
-        <v>0</v>
+        <v>500.779</v>
       </c>
       <c r="F23" s="54">
-        <v>0</v>
+        <v>497.77699999999999</v>
       </c>
       <c r="G23" s="54">
-        <v>0</v>
+        <v>501.40800000000002</v>
       </c>
       <c r="H23" s="54">
-        <v>0</v>
+        <v>508.61700000000002</v>
       </c>
       <c r="I23" s="54">
-        <v>0</v>
+        <v>831.36640000000011</v>
       </c>
       <c r="J23" s="54">
-        <v>0</v>
+        <v>593.13</v>
       </c>
       <c r="K23" s="54">
-        <v>0</v>
+        <v>699.33799999999997</v>
       </c>
       <c r="L23" s="54">
-        <v>0</v>
+        <v>796.60400000000004</v>
       </c>
       <c r="M23" s="54">
-        <v>0</v>
+        <v>877.86599999999999</v>
       </c>
       <c r="N23" s="54">
-        <v>0</v>
+        <v>893.30700000000002</v>
       </c>
       <c r="O23" s="54">
-        <v>0</v>
+        <v>896.11</v>
       </c>
       <c r="P23" s="54">
-        <v>0</v>
+        <v>873.53300000000002</v>
       </c>
       <c r="Q23" s="54">
-        <v>0</v>
+        <v>868.63400000000001</v>
       </c>
       <c r="R23" s="54">
-        <v>0</v>
+        <v>862.76599999999996</v>
       </c>
       <c r="S23" s="54">
-        <v>0</v>
+        <v>787.52700000000004</v>
       </c>
       <c r="T23" s="54">
-        <v>0</v>
+        <v>1678.4111999999998</v>
       </c>
       <c r="U23" s="54">
-        <v>0</v>
+        <v>1572.9659999999999</v>
       </c>
       <c r="V23" s="54">
-        <v>0</v>
+        <v>1539.982</v>
       </c>
       <c r="W23" s="54">
-        <v>0</v>
+        <v>1521.2629999999999</v>
       </c>
       <c r="X23" s="54">
-        <v>0</v>
+        <v>509.49599999999998</v>
       </c>
       <c r="Y23" s="54">
-        <v>0</v>
+        <v>503.91399999999999</v>
       </c>
       <c r="Z23" s="54">
-        <v>0</v>
+        <v>499.52600000000001</v>
       </c>
     </row>
     <row r="24" spans="2:26" x14ac:dyDescent="0.35">
@@ -3336,76 +3336,76 @@
         <v>31</v>
       </c>
       <c r="C33" s="54">
-        <v>506.14800000000002</v>
+        <v>0</v>
       </c>
       <c r="D33" s="54">
-        <v>494.697</v>
+        <v>0</v>
       </c>
       <c r="E33" s="54">
-        <v>500.779</v>
+        <v>0</v>
       </c>
       <c r="F33" s="54">
-        <v>497.77699999999999</v>
+        <v>0</v>
       </c>
       <c r="G33" s="54">
-        <v>501.40800000000002</v>
+        <v>0</v>
       </c>
       <c r="H33" s="54">
-        <v>508.61700000000002</v>
+        <v>0</v>
       </c>
       <c r="I33" s="54">
-        <v>831.36640000000011</v>
+        <v>0</v>
       </c>
       <c r="J33" s="54">
-        <v>593.13</v>
+        <v>0</v>
       </c>
       <c r="K33" s="54">
-        <v>699.33799999999997</v>
+        <v>0</v>
       </c>
       <c r="L33" s="54">
-        <v>796.60400000000004</v>
+        <v>0</v>
       </c>
       <c r="M33" s="54">
-        <v>877.86599999999999</v>
+        <v>0</v>
       </c>
       <c r="N33" s="54">
-        <v>893.30700000000002</v>
+        <v>0</v>
       </c>
       <c r="O33" s="54">
-        <v>896.11</v>
+        <v>0</v>
       </c>
       <c r="P33" s="54">
-        <v>873.53300000000002</v>
+        <v>0</v>
       </c>
       <c r="Q33" s="54">
-        <v>868.63400000000001</v>
+        <v>0</v>
       </c>
       <c r="R33" s="54">
-        <v>862.76599999999996</v>
+        <v>0</v>
       </c>
       <c r="S33" s="54">
-        <v>787.52700000000004</v>
+        <v>0</v>
       </c>
       <c r="T33" s="54">
-        <v>1678.4111999999998</v>
+        <v>0</v>
       </c>
       <c r="U33" s="54">
-        <v>1572.9659999999999</v>
+        <v>0</v>
       </c>
       <c r="V33" s="54">
-        <v>1539.982</v>
+        <v>0</v>
       </c>
       <c r="W33" s="54">
-        <v>1521.2629999999999</v>
+        <v>0</v>
       </c>
       <c r="X33" s="54">
-        <v>509.49599999999998</v>
+        <v>0</v>
       </c>
       <c r="Y33" s="54">
-        <v>503.91399999999999</v>
+        <v>0</v>
       </c>
       <c r="Z33" s="54">
-        <v>499.52600000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="2:26" x14ac:dyDescent="0.35">
@@ -3567,76 +3567,76 @@
         <v>34</v>
       </c>
       <c r="C36" s="54">
-        <v>99.894999999999996</v>
+        <v>77.081639600000003</v>
       </c>
       <c r="D36" s="54">
-        <v>80.106999999999999</v>
+        <v>76.205639599999998</v>
       </c>
       <c r="E36" s="54">
-        <v>67.613</v>
+        <v>77.573806099999999</v>
       </c>
       <c r="F36" s="54">
-        <v>45.598999999999997</v>
+        <v>75.894639600000005</v>
       </c>
       <c r="G36" s="54">
-        <v>41.491</v>
+        <v>76.521139499999904</v>
       </c>
       <c r="H36" s="54">
-        <v>42.502000000000002</v>
+        <v>78.041639599999996</v>
       </c>
       <c r="I36" s="54">
-        <v>82.678400000000011</v>
+        <v>138.90155632000003</v>
       </c>
       <c r="J36" s="54">
-        <v>55.398000000000003</v>
+        <v>107.0398029</v>
       </c>
       <c r="K36" s="54">
-        <v>84.432000000000002</v>
+        <v>141.36430200000001</v>
       </c>
       <c r="L36" s="54">
-        <v>101.02</v>
+        <v>174.7566344</v>
       </c>
       <c r="M36" s="54">
-        <v>104.41</v>
+        <v>176.8601353</v>
       </c>
       <c r="N36" s="54">
-        <v>108.95</v>
+        <v>176.50713210000001</v>
       </c>
       <c r="O36" s="54">
-        <v>117.32599999999999</v>
+        <v>176.68196620000001</v>
       </c>
       <c r="P36" s="54">
-        <v>108.941</v>
+        <v>177.60013069999999</v>
       </c>
       <c r="Q36" s="54">
-        <v>107.072</v>
+        <v>173.07829939999999</v>
       </c>
       <c r="R36" s="54">
-        <v>95.1</v>
+        <v>172.9864657</v>
       </c>
       <c r="S36" s="54">
-        <v>92.683999999999997</v>
+        <v>171.86096659999899</v>
       </c>
       <c r="T36" s="54">
-        <v>135.09120000000001</v>
+        <v>254.45574360000003</v>
       </c>
       <c r="U36" s="54">
-        <v>105.667</v>
+        <v>213.27413530000001</v>
       </c>
       <c r="V36" s="54">
-        <v>102.72499999999999</v>
+        <v>201.42347029999999</v>
       </c>
       <c r="W36" s="54">
-        <v>108.17400000000001</v>
+        <v>193.4893036</v>
       </c>
       <c r="X36" s="54">
-        <v>120.72</v>
+        <v>90.646970199999998</v>
       </c>
       <c r="Y36" s="54">
-        <v>116.45399999999999</v>
+        <v>86.497136900000001</v>
       </c>
       <c r="Z36" s="54">
-        <v>113.819</v>
+        <v>84.372804500000001</v>
       </c>
     </row>
     <row r="37" spans="2:26" x14ac:dyDescent="0.35">
@@ -3875,76 +3875,76 @@
         <v>38</v>
       </c>
       <c r="C40" s="54">
-        <v>0</v>
+        <v>77.081639600000003</v>
       </c>
       <c r="D40" s="54">
-        <v>0</v>
+        <v>76.205639599999998</v>
       </c>
       <c r="E40" s="54">
-        <v>0</v>
+        <v>77.573806099999999</v>
       </c>
       <c r="F40" s="54">
-        <v>0</v>
+        <v>75.894639600000005</v>
       </c>
       <c r="G40" s="54">
-        <v>0</v>
+        <v>76.521139499999904</v>
       </c>
       <c r="H40" s="54">
-        <v>0</v>
+        <v>78.041639599999996</v>
       </c>
       <c r="I40" s="54">
-        <v>0</v>
+        <v>138.90155632000003</v>
       </c>
       <c r="J40" s="54">
-        <v>0</v>
+        <v>107.0398029</v>
       </c>
       <c r="K40" s="54">
-        <v>0</v>
+        <v>141.36430200000001</v>
       </c>
       <c r="L40" s="54">
-        <v>0</v>
+        <v>174.7566344</v>
       </c>
       <c r="M40" s="54">
-        <v>0</v>
+        <v>176.8601353</v>
       </c>
       <c r="N40" s="54">
-        <v>0</v>
+        <v>176.50713210000001</v>
       </c>
       <c r="O40" s="54">
-        <v>0</v>
+        <v>176.68196620000001</v>
       </c>
       <c r="P40" s="54">
-        <v>0</v>
+        <v>177.60013069999999</v>
       </c>
       <c r="Q40" s="54">
-        <v>0</v>
+        <v>173.07829939999999</v>
       </c>
       <c r="R40" s="54">
-        <v>0</v>
+        <v>172.9864657</v>
       </c>
       <c r="S40" s="54">
-        <v>0</v>
+        <v>171.86096659999899</v>
       </c>
       <c r="T40" s="54">
-        <v>0</v>
+        <v>254.45574360000003</v>
       </c>
       <c r="U40" s="54">
-        <v>0</v>
+        <v>213.27413530000001</v>
       </c>
       <c r="V40" s="54">
-        <v>0</v>
+        <v>201.42347029999999</v>
       </c>
       <c r="W40" s="54">
-        <v>0</v>
+        <v>193.4893036</v>
       </c>
       <c r="X40" s="54">
-        <v>0</v>
+        <v>90.646970199999998</v>
       </c>
       <c r="Y40" s="54">
-        <v>0</v>
+        <v>86.497136900000001</v>
       </c>
       <c r="Z40" s="54">
-        <v>0</v>
+        <v>84.372804500000001</v>
       </c>
     </row>
     <row r="41" spans="2:26" x14ac:dyDescent="0.35">
@@ -4038,7 +4038,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6FD6103-A9EE-4309-90E6-57003CAE8224}">
   <dimension ref="B2:Z41"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
@@ -10284,8 +10284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F55E9F5A-A300-40CA-B4B1-E8AE734BE43C}">
   <dimension ref="A2:IE70"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AH61" sqref="AH61:AH66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10421,7 +10421,7 @@
       </c>
     </row>
     <row r="3" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="61" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="11" t="s">
@@ -10455,10 +10455,10 @@
         <v>0</v>
       </c>
       <c r="L3" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M3" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N3" s="13">
         <v>0</v>
@@ -10476,10 +10476,10 @@
         <v>0</v>
       </c>
       <c r="S3" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T3" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U3" s="13">
         <v>0</v>
@@ -10491,7 +10491,7 @@
         <v>0</v>
       </c>
       <c r="X3" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y3" s="13">
         <v>0</v>
@@ -10518,7 +10518,7 @@
         <v>0</v>
       </c>
       <c r="AG3" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH3" s="13">
         <v>0</v>
@@ -10546,7 +10546,7 @@
       </c>
     </row>
     <row r="4" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A4" s="59"/>
+      <c r="A4" s="62"/>
       <c r="B4" s="11" t="s">
         <v>21</v>
       </c>
@@ -10578,10 +10578,10 @@
         <v>0</v>
       </c>
       <c r="L4" s="8">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="M4" s="8">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N4" s="8">
         <v>0</v>
@@ -10599,10 +10599,10 @@
         <v>0</v>
       </c>
       <c r="S4" s="8">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="T4" s="8">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="U4" s="8">
         <v>0</v>
@@ -10614,7 +10614,7 @@
         <v>0</v>
       </c>
       <c r="X4" s="8">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="Y4" s="8">
         <v>0</v>
@@ -10641,7 +10641,7 @@
         <v>0</v>
       </c>
       <c r="AG4" s="8">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="AH4" s="8">
         <v>0</v>
@@ -10669,7 +10669,7 @@
       </c>
     </row>
     <row r="5" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A5" s="59"/>
+      <c r="A5" s="62"/>
       <c r="B5" s="11" t="s">
         <v>22</v>
       </c>
@@ -10701,10 +10701,10 @@
         <v>0</v>
       </c>
       <c r="L5" s="8">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="M5" s="8">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N5" s="8">
         <v>0</v>
@@ -10722,10 +10722,10 @@
         <v>0</v>
       </c>
       <c r="S5" s="8">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="T5" s="8">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="U5" s="8">
         <v>0</v>
@@ -10737,7 +10737,7 @@
         <v>0</v>
       </c>
       <c r="X5" s="8">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="Y5" s="8">
         <v>0</v>
@@ -10764,7 +10764,7 @@
         <v>0</v>
       </c>
       <c r="AG5" s="8">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="AH5" s="8">
         <v>0</v>
@@ -10792,7 +10792,7 @@
       </c>
     </row>
     <row r="6" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A6" s="59"/>
+      <c r="A6" s="62"/>
       <c r="B6" s="11" t="s">
         <v>10</v>
       </c>
@@ -10915,7 +10915,7 @@
       </c>
     </row>
     <row r="7" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A7" s="59"/>
+      <c r="A7" s="62"/>
       <c r="B7" s="11" t="s">
         <v>23</v>
       </c>
@@ -10946,11 +10946,11 @@
       <c r="K7" s="8">
         <v>0</v>
       </c>
-      <c r="L7" s="8">
-        <v>0</v>
-      </c>
-      <c r="M7" s="8">
-        <v>0</v>
+      <c r="L7" s="50">
+        <v>43.048574146662993</v>
+      </c>
+      <c r="M7" s="50">
+        <v>43.048574146662993</v>
       </c>
       <c r="N7" s="8">
         <v>0</v>
@@ -10967,11 +10967,11 @@
       <c r="R7" s="8">
         <v>0</v>
       </c>
-      <c r="S7" s="8">
-        <v>0</v>
-      </c>
-      <c r="T7" s="8">
-        <v>0</v>
+      <c r="S7" s="50">
+        <v>43.048574146662993</v>
+      </c>
+      <c r="T7" s="50">
+        <v>43.048574146662993</v>
       </c>
       <c r="U7" s="8">
         <v>0</v>
@@ -10982,8 +10982,8 @@
       <c r="W7" s="8">
         <v>0</v>
       </c>
-      <c r="X7" s="50">
-        <v>43.048574146662993</v>
+      <c r="X7" s="8">
+        <v>0</v>
       </c>
       <c r="Y7" s="8">
         <v>0</v>
@@ -11010,7 +11010,7 @@
         <v>0</v>
       </c>
       <c r="AG7" s="50">
-        <v>47.739594241691677</v>
+        <v>0</v>
       </c>
       <c r="AH7" s="8">
         <v>0</v>
@@ -11038,7 +11038,7 @@
       </c>
     </row>
     <row r="8" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A8" s="59"/>
+      <c r="A8" s="62"/>
       <c r="B8" s="11" t="s">
         <v>24</v>
       </c>
@@ -11070,10 +11070,10 @@
         <v>0</v>
       </c>
       <c r="L8" s="8">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="M8" s="8">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="N8" s="8">
         <v>0</v>
@@ -11091,10 +11091,10 @@
         <v>0</v>
       </c>
       <c r="S8" s="8">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="T8" s="8">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="U8" s="8">
         <v>0</v>
@@ -11106,7 +11106,7 @@
         <v>0</v>
       </c>
       <c r="X8" s="8">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="Y8" s="8">
         <v>0</v>
@@ -11133,7 +11133,7 @@
         <v>0</v>
       </c>
       <c r="AG8" s="8">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="AH8" s="8">
         <v>0</v>
@@ -11161,7 +11161,7 @@
       </c>
     </row>
     <row r="9" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A9" s="59"/>
+      <c r="A9" s="62"/>
       <c r="B9" s="11" t="s">
         <v>25</v>
       </c>
@@ -11193,10 +11193,10 @@
         <v>0</v>
       </c>
       <c r="L9" s="8">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="M9" s="8">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="N9" s="8">
         <v>0</v>
@@ -11214,10 +11214,10 @@
         <v>0</v>
       </c>
       <c r="S9" s="8">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="T9" s="8">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="U9" s="8">
         <v>0</v>
@@ -11229,7 +11229,7 @@
         <v>0</v>
       </c>
       <c r="X9" s="8">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="Y9" s="8">
         <v>0</v>
@@ -11256,7 +11256,7 @@
         <v>0</v>
       </c>
       <c r="AG9" s="8">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="AH9" s="8">
         <v>0</v>
@@ -11284,7 +11284,7 @@
       </c>
     </row>
     <row r="10" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A10" s="59"/>
+      <c r="A10" s="62"/>
       <c r="B10" s="11" t="s">
         <v>26</v>
       </c>
@@ -11316,10 +11316,10 @@
         <v>0</v>
       </c>
       <c r="L10" s="8">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="M10" s="8">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="N10" s="8">
         <v>0</v>
@@ -11337,10 +11337,10 @@
         <v>0</v>
       </c>
       <c r="S10" s="8">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="T10" s="8">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="U10" s="8">
         <v>0</v>
@@ -11352,7 +11352,7 @@
         <v>0</v>
       </c>
       <c r="X10" s="8">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="Y10" s="8">
         <v>0</v>
@@ -11379,7 +11379,7 @@
         <v>0</v>
       </c>
       <c r="AG10" s="8">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="AH10" s="8">
         <v>0</v>
@@ -11407,7 +11407,7 @@
       </c>
     </row>
     <row r="11" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A11" s="59"/>
+      <c r="A11" s="62"/>
       <c r="B11" s="17" t="s">
         <v>27</v>
       </c>
@@ -11439,10 +11439,10 @@
         <v>0</v>
       </c>
       <c r="L11" s="8">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="M11" s="8">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="N11" s="8">
         <v>0</v>
@@ -11460,10 +11460,10 @@
         <v>0</v>
       </c>
       <c r="S11" s="8">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="T11" s="8">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="U11" s="8">
         <v>0</v>
@@ -11475,7 +11475,7 @@
         <v>0</v>
       </c>
       <c r="X11" s="8">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="Y11" s="8">
         <v>0</v>
@@ -11502,7 +11502,7 @@
         <v>0</v>
       </c>
       <c r="AG11" s="8">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="AH11" s="8">
         <v>0</v>
@@ -11530,7 +11530,7 @@
       </c>
     </row>
     <row r="12" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A12" s="59"/>
+      <c r="A12" s="62"/>
       <c r="B12" s="17" t="s">
         <v>28</v>
       </c>
@@ -11562,10 +11562,10 @@
         <v>0</v>
       </c>
       <c r="L12" s="8">
-        <v>0</v>
+        <v>26.8</v>
       </c>
       <c r="M12" s="8">
-        <v>0</v>
+        <v>26.8</v>
       </c>
       <c r="N12" s="8">
         <v>0</v>
@@ -11583,10 +11583,10 @@
         <v>0</v>
       </c>
       <c r="S12" s="8">
-        <v>0</v>
+        <v>26.8</v>
       </c>
       <c r="T12" s="8">
-        <v>0</v>
+        <v>26.8</v>
       </c>
       <c r="U12" s="8">
         <v>0</v>
@@ -11598,7 +11598,7 @@
         <v>0</v>
       </c>
       <c r="X12" s="8">
-        <v>26.8</v>
+        <v>0</v>
       </c>
       <c r="Y12" s="8">
         <v>0</v>
@@ -11625,7 +11625,7 @@
         <v>0</v>
       </c>
       <c r="AG12" s="8">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="AH12" s="8">
         <v>0</v>
@@ -11653,7 +11653,7 @@
       </c>
     </row>
     <row r="13" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A13" s="59"/>
+      <c r="A13" s="62"/>
       <c r="B13" s="11" t="s">
         <v>29</v>
       </c>
@@ -11685,10 +11685,10 @@
         <v>0</v>
       </c>
       <c r="L13" s="8">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="M13" s="8">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="N13" s="8">
         <v>0</v>
@@ -11706,10 +11706,10 @@
         <v>0</v>
       </c>
       <c r="S13" s="8">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="T13" s="8">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="U13" s="8">
         <v>0</v>
@@ -11721,7 +11721,7 @@
         <v>0</v>
       </c>
       <c r="X13" s="8">
-        <v>56</v>
+        <v>0</v>
       </c>
       <c r="Y13" s="8">
         <v>0</v>
@@ -11748,7 +11748,7 @@
         <v>0</v>
       </c>
       <c r="AG13" s="8">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="AH13" s="8">
         <v>0</v>
@@ -11776,7 +11776,7 @@
       </c>
     </row>
     <row r="14" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A14" s="59"/>
+      <c r="A14" s="62"/>
       <c r="B14" s="17" t="s">
         <v>30</v>
       </c>
@@ -11808,10 +11808,10 @@
         <v>0</v>
       </c>
       <c r="L14" s="8">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="M14" s="8">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="N14" s="8">
         <v>0</v>
@@ -11829,10 +11829,10 @@
         <v>0</v>
       </c>
       <c r="S14" s="8">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="T14" s="8">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="U14" s="8">
         <v>0</v>
@@ -11844,7 +11844,7 @@
         <v>0</v>
       </c>
       <c r="X14" s="8">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="Y14" s="8">
         <v>0</v>
@@ -11871,7 +11871,7 @@
         <v>0</v>
       </c>
       <c r="AG14" s="8">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="AH14" s="8">
         <v>0</v>
@@ -11899,7 +11899,7 @@
       </c>
     </row>
     <row r="15" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A15" s="59"/>
+      <c r="A15" s="62"/>
       <c r="B15" s="11" t="s">
         <v>31</v>
       </c>
@@ -11930,11 +11930,11 @@
       <c r="K15" s="15">
         <v>0</v>
       </c>
-      <c r="L15" s="15">
-        <v>0</v>
-      </c>
-      <c r="M15" s="15">
-        <v>0</v>
+      <c r="L15" s="8">
+        <v>24</v>
+      </c>
+      <c r="M15" s="8">
+        <v>24</v>
       </c>
       <c r="N15" s="15">
         <v>0</v>
@@ -11951,11 +11951,11 @@
       <c r="R15" s="15">
         <v>0</v>
       </c>
-      <c r="S15" s="15">
-        <v>0</v>
-      </c>
-      <c r="T15" s="15">
-        <v>0</v>
+      <c r="S15" s="8">
+        <v>24</v>
+      </c>
+      <c r="T15" s="8">
+        <v>24</v>
       </c>
       <c r="U15" s="15">
         <v>0</v>
@@ -11966,8 +11966,8 @@
       <c r="W15" s="15">
         <v>0</v>
       </c>
-      <c r="X15" s="8">
-        <v>24</v>
+      <c r="X15" s="15">
+        <v>0</v>
       </c>
       <c r="Y15" s="15">
         <v>0</v>
@@ -11994,7 +11994,7 @@
         <v>0</v>
       </c>
       <c r="AG15" s="8">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="AH15" s="8">
         <v>0</v>
@@ -12022,7 +12022,7 @@
       </c>
     </row>
     <row r="16" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A16" s="58" t="s">
+      <c r="A16" s="61" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="12" t="s">
@@ -12147,7 +12147,7 @@
       </c>
     </row>
     <row r="17" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A17" s="59"/>
+      <c r="A17" s="62"/>
       <c r="B17" s="11" t="s">
         <v>13</v>
       </c>
@@ -12270,7 +12270,7 @@
       </c>
     </row>
     <row r="18" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A18" s="59"/>
+      <c r="A18" s="62"/>
       <c r="B18" s="11" t="s">
         <v>14</v>
       </c>
@@ -12393,7 +12393,7 @@
       </c>
     </row>
     <row r="19" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A19" s="59"/>
+      <c r="A19" s="62"/>
       <c r="B19" s="11" t="s">
         <v>15</v>
       </c>
@@ -12516,7 +12516,7 @@
       </c>
     </row>
     <row r="20" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A20" s="59"/>
+      <c r="A20" s="62"/>
       <c r="B20" s="17" t="s">
         <v>16</v>
       </c>
@@ -12639,7 +12639,7 @@
       </c>
     </row>
     <row r="21" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A21" s="59"/>
+      <c r="A21" s="62"/>
       <c r="B21" s="17" t="s">
         <v>17</v>
       </c>
@@ -12762,7 +12762,7 @@
       </c>
     </row>
     <row r="22" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A22" s="59"/>
+      <c r="A22" s="62"/>
       <c r="B22" s="17" t="s">
         <v>19</v>
       </c>
@@ -12885,7 +12885,7 @@
       </c>
     </row>
     <row r="23" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A23" s="59"/>
+      <c r="A23" s="62"/>
       <c r="B23" s="17" t="s">
         <v>20</v>
       </c>
@@ -13008,7 +13008,7 @@
       </c>
     </row>
     <row r="24" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A24" s="60"/>
+      <c r="A24" s="63"/>
       <c r="B24" s="16" t="s">
         <v>18</v>
       </c>
@@ -13131,7 +13131,7 @@
       </c>
     </row>
     <row r="25" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A25" s="58" t="s">
+      <c r="A25" s="61" t="s">
         <v>1</v>
       </c>
       <c r="B25" s="11" t="s">
@@ -13141,7 +13141,7 @@
         <v>1</v>
       </c>
       <c r="D25" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E25" s="13">
         <v>0</v>
@@ -13168,10 +13168,10 @@
         <v>0</v>
       </c>
       <c r="M25" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N25" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O25" s="13">
         <v>0</v>
@@ -13183,7 +13183,7 @@
         <v>0</v>
       </c>
       <c r="R25" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S25" s="13">
         <v>0</v>
@@ -13198,7 +13198,7 @@
         <v>0</v>
       </c>
       <c r="W25" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X25" s="13">
         <v>0</v>
@@ -13207,7 +13207,7 @@
         <v>0</v>
       </c>
       <c r="Z25" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA25" s="13">
         <v>0</v>
@@ -13225,16 +13225,16 @@
         <v>0</v>
       </c>
       <c r="AF25" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG25" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH25" s="13">
         <v>0</v>
       </c>
       <c r="AI25" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ25" s="13">
         <v>1</v>
@@ -13252,11 +13252,11 @@
         <v>1</v>
       </c>
       <c r="AO25" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A26" s="60"/>
+      <c r="A26" s="63"/>
       <c r="B26" s="14" t="s">
         <v>3</v>
       </c>
@@ -13264,7 +13264,7 @@
         <v>9</v>
       </c>
       <c r="D26" s="15">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E26" s="15">
         <v>0</v>
@@ -13291,10 +13291,10 @@
         <v>0</v>
       </c>
       <c r="M26" s="15">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="N26" s="15">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="O26" s="15">
         <v>0</v>
@@ -13306,7 +13306,7 @@
         <v>0</v>
       </c>
       <c r="R26" s="15">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="S26" s="15">
         <v>0</v>
@@ -13321,65 +13321,65 @@
         <v>0</v>
       </c>
       <c r="W26" s="15">
+        <v>0</v>
+      </c>
+      <c r="X26" s="15">
+        <v>0</v>
+      </c>
+      <c r="Y26" s="15">
+        <v>0</v>
+      </c>
+      <c r="Z26" s="15">
+        <v>0</v>
+      </c>
+      <c r="AA26" s="15">
+        <v>0</v>
+      </c>
+      <c r="AB26" s="15">
+        <v>0</v>
+      </c>
+      <c r="AC26" s="15">
+        <v>0</v>
+      </c>
+      <c r="AD26" s="15">
+        <v>0</v>
+      </c>
+      <c r="AE26" s="15">
+        <v>0</v>
+      </c>
+      <c r="AF26" s="15">
+        <v>9</v>
+      </c>
+      <c r="AG26" s="15">
+        <v>0</v>
+      </c>
+      <c r="AH26" s="15">
+        <v>0</v>
+      </c>
+      <c r="AI26" s="15">
+        <v>0</v>
+      </c>
+      <c r="AJ26" s="15">
+        <v>19</v>
+      </c>
+      <c r="AK26" s="15">
+        <v>0</v>
+      </c>
+      <c r="AL26" s="15">
+        <v>0</v>
+      </c>
+      <c r="AM26" s="15">
+        <v>0</v>
+      </c>
+      <c r="AN26" s="15">
         <v>20</v>
       </c>
-      <c r="X26" s="15">
-        <v>0</v>
-      </c>
-      <c r="Y26" s="15">
-        <v>0</v>
-      </c>
-      <c r="Z26" s="15">
-        <v>18</v>
-      </c>
-      <c r="AA26" s="15">
-        <v>0</v>
-      </c>
-      <c r="AB26" s="15">
-        <v>0</v>
-      </c>
-      <c r="AC26" s="15">
-        <v>0</v>
-      </c>
-      <c r="AD26" s="15">
-        <v>0</v>
-      </c>
-      <c r="AE26" s="15">
-        <v>0</v>
-      </c>
-      <c r="AF26" s="15">
-        <v>0</v>
-      </c>
-      <c r="AG26" s="15">
-        <v>9</v>
-      </c>
-      <c r="AH26" s="15">
-        <v>0</v>
-      </c>
-      <c r="AI26" s="15">
-        <v>12</v>
-      </c>
-      <c r="AJ26" s="15">
-        <v>19</v>
-      </c>
-      <c r="AK26" s="15">
-        <v>0</v>
-      </c>
-      <c r="AL26" s="15">
-        <v>0</v>
-      </c>
-      <c r="AM26" s="15">
-        <v>0</v>
-      </c>
-      <c r="AN26" s="15">
-        <v>19</v>
-      </c>
       <c r="AO26" s="15">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A27" s="58" t="s">
+      <c r="A27" s="61" t="s">
         <v>2</v>
       </c>
       <c r="B27" s="12" t="s">
@@ -13504,7 +13504,7 @@
       </c>
     </row>
     <row r="28" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A28" s="59"/>
+      <c r="A28" s="62"/>
       <c r="B28" s="11" t="s">
         <v>3</v>
       </c>
@@ -13535,7 +13535,7 @@
       <c r="K28" s="8">
         <v>0</v>
       </c>
-      <c r="L28" s="61">
+      <c r="L28" s="55">
         <v>15</v>
       </c>
       <c r="M28" s="8">
@@ -13562,7 +13562,7 @@
       <c r="T28" s="8">
         <v>0</v>
       </c>
-      <c r="U28" s="61">
+      <c r="U28" s="55">
         <v>20</v>
       </c>
       <c r="V28" s="8">
@@ -13610,7 +13610,7 @@
       <c r="AJ28" s="8">
         <v>0</v>
       </c>
-      <c r="AK28" s="61">
+      <c r="AK28" s="55">
         <v>20</v>
       </c>
       <c r="AL28" s="8">
@@ -13627,7 +13627,7 @@
       </c>
     </row>
     <row r="29" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A29" s="59"/>
+      <c r="A29" s="62"/>
       <c r="B29" s="11" t="s">
         <v>10</v>
       </c>
@@ -13658,7 +13658,7 @@
       <c r="K29" s="8">
         <v>0</v>
       </c>
-      <c r="L29" s="61">
+      <c r="L29" s="55">
         <v>2</v>
       </c>
       <c r="M29" s="8">
@@ -13685,7 +13685,7 @@
       <c r="T29" s="8">
         <v>0</v>
       </c>
-      <c r="U29" s="61">
+      <c r="U29" s="55">
         <v>2</v>
       </c>
       <c r="V29" s="8">
@@ -13733,7 +13733,7 @@
       <c r="AJ29" s="8">
         <v>0</v>
       </c>
-      <c r="AK29" s="61">
+      <c r="AK29" s="55">
         <v>2</v>
       </c>
       <c r="AL29" s="8">
@@ -13750,7 +13750,7 @@
       </c>
     </row>
     <row r="30" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A30" s="59"/>
+      <c r="A30" s="62"/>
       <c r="B30" s="11" t="s">
         <v>5</v>
       </c>
@@ -13781,7 +13781,7 @@
       <c r="K30" s="8">
         <v>0</v>
       </c>
-      <c r="L30" s="61">
+      <c r="L30" s="55">
         <v>50</v>
       </c>
       <c r="M30" s="8">
@@ -13808,7 +13808,7 @@
       <c r="T30" s="8">
         <v>0</v>
       </c>
-      <c r="U30" s="61">
+      <c r="U30" s="55">
         <v>75</v>
       </c>
       <c r="V30" s="8">
@@ -13856,7 +13856,7 @@
       <c r="AJ30" s="8">
         <v>0</v>
       </c>
-      <c r="AK30" s="61">
+      <c r="AK30" s="55">
         <v>75</v>
       </c>
       <c r="AL30" s="8">
@@ -13873,7 +13873,7 @@
       </c>
     </row>
     <row r="31" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A31" s="59"/>
+      <c r="A31" s="62"/>
       <c r="B31" s="11" t="s">
         <v>8</v>
       </c>
@@ -13904,7 +13904,7 @@
       <c r="K31" s="8">
         <v>0</v>
       </c>
-      <c r="L31" s="61">
+      <c r="L31" s="55">
         <v>5</v>
       </c>
       <c r="M31" s="8">
@@ -13931,7 +13931,7 @@
       <c r="T31" s="8">
         <v>0</v>
       </c>
-      <c r="U31" s="61">
+      <c r="U31" s="55">
         <v>7.5</v>
       </c>
       <c r="V31" s="8">
@@ -13979,7 +13979,7 @@
       <c r="AJ31" s="8">
         <v>0</v>
       </c>
-      <c r="AK31" s="61">
+      <c r="AK31" s="55">
         <v>7.5</v>
       </c>
       <c r="AL31" s="8">
@@ -13996,7 +13996,7 @@
       </c>
     </row>
     <row r="32" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A32" s="59"/>
+      <c r="A32" s="62"/>
       <c r="B32" s="11" t="s">
         <v>6</v>
       </c>
@@ -14027,7 +14027,7 @@
       <c r="K32" s="8">
         <v>0</v>
       </c>
-      <c r="L32" s="61">
+      <c r="L32" s="55">
         <v>25</v>
       </c>
       <c r="M32" s="8">
@@ -14054,7 +14054,7 @@
       <c r="T32" s="8">
         <v>0</v>
       </c>
-      <c r="U32" s="61">
+      <c r="U32" s="55">
         <v>25</v>
       </c>
       <c r="V32" s="8">
@@ -14102,7 +14102,7 @@
       <c r="AJ32" s="8">
         <v>0</v>
       </c>
-      <c r="AK32" s="61">
+      <c r="AK32" s="55">
         <v>25</v>
       </c>
       <c r="AL32" s="8">
@@ -14119,7 +14119,7 @@
       </c>
     </row>
     <row r="33" spans="1:239" x14ac:dyDescent="0.35">
-      <c r="A33" s="60"/>
+      <c r="A33" s="63"/>
       <c r="B33" s="14" t="s">
         <v>7</v>
       </c>
@@ -14150,7 +14150,7 @@
       <c r="K33" s="15">
         <v>0</v>
       </c>
-      <c r="L33" s="62">
+      <c r="L33" s="56">
         <v>0.9</v>
       </c>
       <c r="M33" s="15">
@@ -14177,7 +14177,7 @@
       <c r="T33" s="15">
         <v>0</v>
       </c>
-      <c r="U33" s="62">
+      <c r="U33" s="56">
         <v>0.9</v>
       </c>
       <c r="V33" s="15">
@@ -14225,7 +14225,7 @@
       <c r="AJ33" s="15">
         <v>0</v>
       </c>
-      <c r="AK33" s="62">
+      <c r="AK33" s="56">
         <v>0.9</v>
       </c>
       <c r="AL33" s="15">
@@ -14242,7 +14242,7 @@
       </c>
     </row>
     <row r="34" spans="1:239" x14ac:dyDescent="0.35">
-      <c r="A34" s="58" t="s">
+      <c r="A34" s="61" t="s">
         <v>32</v>
       </c>
       <c r="B34" s="12" t="s">
@@ -14367,7 +14367,7 @@
       </c>
     </row>
     <row r="35" spans="1:239" x14ac:dyDescent="0.35">
-      <c r="A35" s="59"/>
+      <c r="A35" s="62"/>
       <c r="B35" s="11" t="s">
         <v>3</v>
       </c>
@@ -14490,7 +14490,7 @@
       </c>
     </row>
     <row r="36" spans="1:239" x14ac:dyDescent="0.35">
-      <c r="A36" s="59"/>
+      <c r="A36" s="62"/>
       <c r="B36" s="11" t="s">
         <v>33</v>
       </c>
@@ -14613,7 +14613,7 @@
       </c>
     </row>
     <row r="37" spans="1:239" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="60"/>
+      <c r="A37" s="63"/>
       <c r="B37" s="14" t="s">
         <v>7</v>
       </c>
@@ -14736,7 +14736,7 @@
       </c>
     </row>
     <row r="38" spans="1:239" s="20" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="58" t="s">
+      <c r="A38" s="61" t="s">
         <v>34</v>
       </c>
       <c r="B38" s="11" t="s">
@@ -14779,7 +14779,7 @@
         <v>0</v>
       </c>
       <c r="O38" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P38" s="8">
         <v>0</v>
@@ -15059,7 +15059,7 @@
       <c r="IE38" s="10"/>
     </row>
     <row r="39" spans="1:239" x14ac:dyDescent="0.35">
-      <c r="A39" s="59"/>
+      <c r="A39" s="62"/>
       <c r="B39" s="11" t="s">
         <v>3</v>
       </c>
@@ -15100,7 +15100,7 @@
         <v>0</v>
       </c>
       <c r="O39" s="8">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="P39" s="8">
         <v>0</v>
@@ -15182,7 +15182,7 @@
       </c>
     </row>
     <row r="40" spans="1:239" s="19" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="60"/>
+      <c r="A40" s="63"/>
       <c r="B40" s="14" t="s">
         <v>7</v>
       </c>
@@ -15223,7 +15223,7 @@
         <v>0</v>
       </c>
       <c r="O40" s="8">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="P40" s="8">
         <v>0</v>
@@ -15503,7 +15503,7 @@
       <c r="IE40" s="10"/>
     </row>
     <row r="41" spans="1:239" x14ac:dyDescent="0.35">
-      <c r="A41" s="58" t="s">
+      <c r="A41" s="61" t="s">
         <v>35</v>
       </c>
       <c r="B41" s="12" t="s">
@@ -15543,7 +15543,7 @@
         <v>0</v>
       </c>
       <c r="N41" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O41" s="13">
         <v>0</v>
@@ -15555,13 +15555,13 @@
         <v>0</v>
       </c>
       <c r="R41" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S41" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T41" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U41" s="13">
         <v>0</v>
@@ -15570,7 +15570,7 @@
         <v>0</v>
       </c>
       <c r="W41" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X41" s="13">
         <v>0</v>
@@ -15609,7 +15609,7 @@
         <v>0</v>
       </c>
       <c r="AJ41" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK41" s="13">
         <v>0</v>
@@ -15628,7 +15628,7 @@
       </c>
     </row>
     <row r="42" spans="1:239" x14ac:dyDescent="0.35">
-      <c r="A42" s="59"/>
+      <c r="A42" s="62"/>
       <c r="B42" s="11" t="s">
         <v>36</v>
       </c>
@@ -15666,7 +15666,7 @@
         <v>0</v>
       </c>
       <c r="N42" s="8">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="O42" s="8">
         <v>0</v>
@@ -15678,23 +15678,23 @@
         <v>0</v>
       </c>
       <c r="R42" s="8">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="S42" s="8">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="T42" s="8">
+        <v>0</v>
+      </c>
+      <c r="U42" s="8">
+        <v>0</v>
+      </c>
+      <c r="V42" s="8">
+        <v>0</v>
+      </c>
+      <c r="W42" s="8">
         <v>150</v>
       </c>
-      <c r="U42" s="8">
-        <v>0</v>
-      </c>
-      <c r="V42" s="8">
-        <v>0</v>
-      </c>
-      <c r="W42" s="8">
-        <v>0</v>
-      </c>
       <c r="X42" s="8">
         <v>0</v>
       </c>
@@ -15732,7 +15732,7 @@
         <v>0</v>
       </c>
       <c r="AJ42" s="8">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="AK42" s="8">
         <v>0</v>
@@ -15751,7 +15751,7 @@
       </c>
     </row>
     <row r="43" spans="1:239" x14ac:dyDescent="0.35">
-      <c r="A43" s="59"/>
+      <c r="A43" s="62"/>
       <c r="B43" s="17" t="s">
         <v>37</v>
       </c>
@@ -15789,7 +15789,7 @@
         <v>0</v>
       </c>
       <c r="N43" s="8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O43" s="8">
         <v>0</v>
@@ -15801,23 +15801,23 @@
         <v>0</v>
       </c>
       <c r="R43" s="8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S43" s="8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T43" s="8">
+        <v>0</v>
+      </c>
+      <c r="U43" s="8">
+        <v>0</v>
+      </c>
+      <c r="V43" s="8">
+        <v>0</v>
+      </c>
+      <c r="W43" s="8">
         <v>3</v>
       </c>
-      <c r="U43" s="8">
-        <v>0</v>
-      </c>
-      <c r="V43" s="8">
-        <v>0</v>
-      </c>
-      <c r="W43" s="8">
-        <v>0</v>
-      </c>
       <c r="X43" s="8">
         <v>0</v>
       </c>
@@ -15855,7 +15855,7 @@
         <v>0</v>
       </c>
       <c r="AJ43" s="8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AK43" s="8">
         <v>0</v>
@@ -15874,7 +15874,7 @@
       </c>
     </row>
     <row r="44" spans="1:239" x14ac:dyDescent="0.35">
-      <c r="A44" s="59"/>
+      <c r="A44" s="62"/>
       <c r="B44" s="17" t="s">
         <v>38</v>
       </c>
@@ -15912,7 +15912,7 @@
         <v>0</v>
       </c>
       <c r="N44" s="8">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="O44" s="8">
         <v>0</v>
@@ -15924,23 +15924,23 @@
         <v>0</v>
       </c>
       <c r="R44" s="8">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="S44" s="8">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="T44" s="8">
+        <v>0</v>
+      </c>
+      <c r="U44" s="8">
+        <v>0</v>
+      </c>
+      <c r="V44" s="8">
+        <v>0</v>
+      </c>
+      <c r="W44" s="8">
         <v>10</v>
       </c>
-      <c r="U44" s="8">
-        <v>0</v>
-      </c>
-      <c r="V44" s="8">
-        <v>0</v>
-      </c>
-      <c r="W44" s="8">
-        <v>0</v>
-      </c>
       <c r="X44" s="8">
         <v>0</v>
       </c>
@@ -15978,7 +15978,7 @@
         <v>0</v>
       </c>
       <c r="AJ44" s="8">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AK44" s="8">
         <v>0</v>
@@ -15997,7 +15997,7 @@
       </c>
     </row>
     <row r="45" spans="1:239" x14ac:dyDescent="0.35">
-      <c r="A45" s="60"/>
+      <c r="A45" s="63"/>
       <c r="B45" s="14" t="s">
         <v>39</v>
       </c>
@@ -16035,7 +16035,7 @@
         <v>0</v>
       </c>
       <c r="N45" s="15">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="O45" s="15">
         <v>0</v>
@@ -16047,23 +16047,23 @@
         <v>0</v>
       </c>
       <c r="R45" s="15">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="S45" s="15">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="T45" s="15">
+        <v>0</v>
+      </c>
+      <c r="U45" s="15">
+        <v>0</v>
+      </c>
+      <c r="V45" s="15">
+        <v>0</v>
+      </c>
+      <c r="W45" s="15">
         <v>26</v>
       </c>
-      <c r="U45" s="15">
-        <v>0</v>
-      </c>
-      <c r="V45" s="15">
-        <v>0</v>
-      </c>
-      <c r="W45" s="15">
-        <v>0</v>
-      </c>
       <c r="X45" s="15">
         <v>0</v>
       </c>
@@ -16101,7 +16101,7 @@
         <v>0</v>
       </c>
       <c r="AJ45" s="15">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AK45" s="15">
         <v>0</v>
@@ -16120,7 +16120,7 @@
       </c>
     </row>
     <row r="46" spans="1:239" x14ac:dyDescent="0.35">
-      <c r="A46" s="58" t="s">
+      <c r="A46" s="61" t="s">
         <v>40</v>
       </c>
       <c r="B46" s="12" t="s">
@@ -16169,7 +16169,7 @@
         <v>0</v>
       </c>
       <c r="Q46" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R46" s="13">
         <v>0</v>
@@ -16187,7 +16187,7 @@
         <v>0</v>
       </c>
       <c r="W46" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X46" s="13">
         <v>0</v>
@@ -16214,7 +16214,7 @@
         <v>0</v>
       </c>
       <c r="AF46" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG46" s="13">
         <v>0</v>
@@ -16245,7 +16245,7 @@
       </c>
     </row>
     <row r="47" spans="1:239" x14ac:dyDescent="0.35">
-      <c r="A47" s="59"/>
+      <c r="A47" s="62"/>
       <c r="B47" s="11" t="s">
         <v>44</v>
       </c>
@@ -16292,7 +16292,7 @@
         <v>0</v>
       </c>
       <c r="Q47" s="8">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="R47" s="8">
         <v>0</v>
@@ -16310,7 +16310,7 @@
         <v>0</v>
       </c>
       <c r="W47" s="8">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="X47" s="8">
         <v>0</v>
@@ -16337,7 +16337,7 @@
         <v>0</v>
       </c>
       <c r="AF47" s="8">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="AG47" s="8">
         <v>0</v>
@@ -16368,7 +16368,7 @@
       </c>
     </row>
     <row r="48" spans="1:239" x14ac:dyDescent="0.35">
-      <c r="A48" s="59"/>
+      <c r="A48" s="62"/>
       <c r="B48" s="11" t="s">
         <v>45</v>
       </c>
@@ -16415,7 +16415,7 @@
         <v>0</v>
       </c>
       <c r="Q48" s="8">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="R48" s="8">
         <v>0</v>
@@ -16433,7 +16433,7 @@
         <v>0</v>
       </c>
       <c r="W48" s="8">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="X48" s="8">
         <v>0</v>
@@ -16460,7 +16460,7 @@
         <v>0</v>
       </c>
       <c r="AF48" s="8">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AG48" s="8">
         <v>0</v>
@@ -16491,7 +16491,7 @@
       </c>
     </row>
     <row r="49" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A49" s="59"/>
+      <c r="A49" s="62"/>
       <c r="B49" s="17" t="s">
         <v>41</v>
       </c>
@@ -16538,7 +16538,7 @@
         <v>0</v>
       </c>
       <c r="Q49" s="8">
-        <v>0.85</v>
+        <v>0</v>
       </c>
       <c r="R49" s="8">
         <v>0</v>
@@ -16556,7 +16556,7 @@
         <v>0</v>
       </c>
       <c r="W49" s="8">
-        <v>0.85</v>
+        <v>0</v>
       </c>
       <c r="X49" s="8">
         <v>0</v>
@@ -16583,7 +16583,7 @@
         <v>0</v>
       </c>
       <c r="AF49" s="8">
-        <v>0.85</v>
+        <v>0</v>
       </c>
       <c r="AG49" s="8">
         <v>0</v>
@@ -16614,7 +16614,7 @@
       </c>
     </row>
     <row r="50" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A50" s="59"/>
+      <c r="A50" s="62"/>
       <c r="B50" s="17" t="s">
         <v>42</v>
       </c>
@@ -16661,7 +16661,7 @@
         <v>0</v>
       </c>
       <c r="Q50" s="8">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="R50" s="8">
         <v>0</v>
@@ -16679,7 +16679,7 @@
         <v>0</v>
       </c>
       <c r="W50" s="8">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="X50" s="8">
         <v>0</v>
@@ -16706,7 +16706,7 @@
         <v>0</v>
       </c>
       <c r="AF50" s="8">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="AG50" s="8">
         <v>0</v>
@@ -16737,7 +16737,7 @@
       </c>
     </row>
     <row r="51" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A51" s="60"/>
+      <c r="A51" s="63"/>
       <c r="B51" s="17" t="s">
         <v>43</v>
       </c>
@@ -16784,7 +16784,7 @@
         <v>0</v>
       </c>
       <c r="Q51" s="15">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="R51" s="15">
         <v>0</v>
@@ -16802,7 +16802,7 @@
         <v>0</v>
       </c>
       <c r="W51" s="15">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="X51" s="15">
         <v>0</v>
@@ -16829,7 +16829,7 @@
         <v>0</v>
       </c>
       <c r="AF51" s="15">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="AG51" s="15">
         <v>0</v>
@@ -16860,7 +16860,7 @@
       </c>
     </row>
     <row r="52" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A52" s="58" t="s">
+      <c r="A52" s="61" t="s">
         <v>64</v>
       </c>
       <c r="B52" s="12" t="s">
@@ -16985,7 +16985,7 @@
       </c>
     </row>
     <row r="53" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A53" s="59"/>
+      <c r="A53" s="62"/>
       <c r="B53" s="31" t="s">
         <v>59</v>
       </c>
@@ -17080,7 +17080,7 @@
         <v>8.715947912047902</v>
       </c>
       <c r="AG53" s="51">
-        <v>33.067446572522428</v>
+        <v>8.715947912047902</v>
       </c>
       <c r="AH53" s="51">
         <v>14.100746968028449</v>
@@ -17108,7 +17108,7 @@
       </c>
     </row>
     <row r="54" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A54" s="59"/>
+      <c r="A54" s="62"/>
       <c r="B54" s="31" t="s">
         <v>60</v>
       </c>
@@ -17203,7 +17203,7 @@
         <v>0.73110699540728952</v>
       </c>
       <c r="AG54" s="51">
-        <v>3.5593495034616041</v>
+        <v>0.73110699540728952</v>
       </c>
       <c r="AH54" s="51">
         <v>2.8939587848196382</v>
@@ -17231,7 +17231,7 @@
       </c>
     </row>
     <row r="55" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A55" s="59"/>
+      <c r="A55" s="62"/>
       <c r="B55" s="31" t="s">
         <v>61</v>
       </c>
@@ -17354,7 +17354,7 @@
       </c>
     </row>
     <row r="56" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A56" s="59"/>
+      <c r="A56" s="62"/>
       <c r="B56" s="32" t="s">
         <v>62</v>
       </c>
@@ -17477,7 +17477,7 @@
       </c>
     </row>
     <row r="57" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A57" s="59"/>
+      <c r="A57" s="62"/>
       <c r="B57" s="32" t="s">
         <v>63</v>
       </c>
@@ -17600,130 +17600,130 @@
       </c>
     </row>
     <row r="58" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A58" s="59"/>
+      <c r="A58" s="62"/>
       <c r="B58" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="C58" s="63">
+      <c r="C58" s="57">
         <v>28.642165487</v>
       </c>
-      <c r="D58" s="63">
+      <c r="D58" s="57">
         <v>13.709839065000001</v>
       </c>
-      <c r="E58" s="63">
+      <c r="E58" s="57">
         <v>17.116117564</v>
       </c>
-      <c r="F58" s="63">
+      <c r="F58" s="57">
         <v>20.047835054</v>
       </c>
-      <c r="G58" s="63">
+      <c r="G58" s="57">
         <v>48.813144185000013</v>
       </c>
-      <c r="H58" s="63">
+      <c r="H58" s="57">
         <v>48.597325439000002</v>
       </c>
-      <c r="I58" s="63">
+      <c r="I58" s="57">
         <v>71.115404463999994</v>
       </c>
-      <c r="J58" s="63">
+      <c r="J58" s="57">
         <v>14.86170413</v>
       </c>
-      <c r="K58" s="63">
+      <c r="K58" s="57">
         <v>20.076718505999999</v>
       </c>
-      <c r="L58" s="63">
+      <c r="L58" s="57">
         <v>17.593506775000002</v>
       </c>
-      <c r="M58" s="63">
+      <c r="M58" s="57">
         <v>85.343995515999993</v>
       </c>
-      <c r="N58" s="63">
+      <c r="N58" s="57">
         <v>13.5071625</v>
       </c>
-      <c r="O58" s="63">
+      <c r="O58" s="57">
         <v>15.383693883999999</v>
       </c>
-      <c r="P58" s="63">
+      <c r="P58" s="57">
         <v>41.343083131999997</v>
       </c>
-      <c r="Q58" s="63">
+      <c r="Q58" s="57">
         <v>45.075177836000002</v>
       </c>
-      <c r="R58" s="63">
+      <c r="R58" s="57">
         <v>44.822247808000007</v>
       </c>
-      <c r="S58" s="63">
+      <c r="S58" s="57">
         <v>33.070377391999997</v>
       </c>
-      <c r="T58" s="63">
+      <c r="T58" s="57">
         <v>22.249291466999999</v>
       </c>
-      <c r="U58" s="63">
+      <c r="U58" s="57">
         <v>25.794705144000002</v>
       </c>
-      <c r="V58" s="63">
+      <c r="V58" s="57">
         <v>33.737642405999999</v>
       </c>
-      <c r="W58" s="63">
+      <c r="W58" s="57">
         <v>19.780558303999999</v>
       </c>
-      <c r="X58" s="63">
+      <c r="X58" s="57">
         <v>51.402821756000002</v>
       </c>
-      <c r="Y58" s="63">
+      <c r="Y58" s="57">
         <v>33.864090234000003</v>
       </c>
-      <c r="Z58" s="63">
+      <c r="Z58" s="57">
         <v>29.129919520000001</v>
       </c>
-      <c r="AA58" s="63">
+      <c r="AA58" s="57">
         <v>24.819653352</v>
       </c>
-      <c r="AB58" s="63">
+      <c r="AB58" s="57">
         <v>16.137710160000001</v>
       </c>
-      <c r="AC58" s="63">
+      <c r="AC58" s="57">
         <v>42.757859105000009</v>
       </c>
-      <c r="AD58" s="63">
+      <c r="AD58" s="57">
         <v>22.620722240999999</v>
       </c>
-      <c r="AE58" s="63">
+      <c r="AE58" s="57">
         <v>20.323116593000002</v>
       </c>
-      <c r="AF58" s="63">
+      <c r="AF58" s="57">
         <v>74.025039647</v>
       </c>
-      <c r="AG58" s="63">
-        <v>19.924262202000001</v>
-      </c>
-      <c r="AH58" s="63">
+      <c r="AG58" s="57">
+        <v>74.025039647</v>
+      </c>
+      <c r="AH58" s="57">
         <v>46.626702238999997</v>
       </c>
-      <c r="AI58" s="63">
+      <c r="AI58" s="57">
         <v>68.383762524999995</v>
       </c>
-      <c r="AJ58" s="63">
+      <c r="AJ58" s="57">
         <v>13.702268788</v>
       </c>
-      <c r="AK58" s="63">
+      <c r="AK58" s="57">
         <v>13.557096163000001</v>
       </c>
-      <c r="AL58" s="63">
+      <c r="AL58" s="57">
         <v>15.766890009000001</v>
       </c>
-      <c r="AM58" s="63">
+      <c r="AM58" s="57">
         <v>33.032526019999999</v>
       </c>
-      <c r="AN58" s="63">
+      <c r="AN58" s="57">
         <v>60.047136006000002</v>
       </c>
-      <c r="AO58" s="63">
+      <c r="AO58" s="57">
         <v>18.033061254</v>
       </c>
     </row>
     <row r="59" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A59" s="59"/>
+      <c r="A59" s="62"/>
       <c r="B59" s="17" t="s">
         <v>47</v>
       </c>
@@ -17846,7 +17846,7 @@
       </c>
     </row>
     <row r="60" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A60" s="60"/>
+      <c r="A60" s="63"/>
       <c r="B60" s="18" t="s">
         <v>48</v>
       </c>
@@ -17941,7 +17941,7 @@
         <v>4.7511102277086099</v>
       </c>
       <c r="AG60" s="53">
-        <v>4.645759633098324</v>
+        <v>4.7511102277086099</v>
       </c>
       <c r="AH60" s="53">
         <v>4.615395981965758</v>
@@ -17969,7 +17969,7 @@
       </c>
     </row>
     <row r="61" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A61" s="55" t="s">
+      <c r="A61" s="58" t="s">
         <v>11</v>
       </c>
       <c r="B61" s="12" t="s">
@@ -18030,7 +18030,7 @@
         <v>0</v>
       </c>
       <c r="U61" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V61" s="8">
         <v>0</v>
@@ -18090,11 +18090,11 @@
         <v>0</v>
       </c>
       <c r="AO61" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A62" s="56"/>
+      <c r="A62" s="59"/>
       <c r="B62" s="17" t="s">
         <v>49</v>
       </c>
@@ -18153,71 +18153,71 @@
         <v>0</v>
       </c>
       <c r="U62" s="8">
+        <v>0</v>
+      </c>
+      <c r="V62" s="8">
+        <v>0</v>
+      </c>
+      <c r="W62" s="8">
+        <v>0</v>
+      </c>
+      <c r="X62" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y62" s="8">
+        <v>0</v>
+      </c>
+      <c r="Z62" s="8">
+        <v>0</v>
+      </c>
+      <c r="AA62" s="8">
+        <v>0</v>
+      </c>
+      <c r="AB62" s="8">
+        <v>0</v>
+      </c>
+      <c r="AC62" s="8">
+        <v>0</v>
+      </c>
+      <c r="AD62" s="8">
+        <v>0</v>
+      </c>
+      <c r="AE62" s="8">
+        <v>0</v>
+      </c>
+      <c r="AF62" s="8">
+        <v>0</v>
+      </c>
+      <c r="AG62" s="8">
+        <v>0</v>
+      </c>
+      <c r="AH62" s="8">
+        <v>0</v>
+      </c>
+      <c r="AI62" s="8">
+        <v>0</v>
+      </c>
+      <c r="AJ62" s="8">
+        <v>0</v>
+      </c>
+      <c r="AK62" s="8">
+        <v>0</v>
+      </c>
+      <c r="AL62" s="8">
+        <v>0</v>
+      </c>
+      <c r="AM62" s="8">
+        <v>0</v>
+      </c>
+      <c r="AN62" s="8">
+        <v>0</v>
+      </c>
+      <c r="AO62" s="8">
         <v>200</v>
       </c>
-      <c r="V62" s="8">
-        <v>0</v>
-      </c>
-      <c r="W62" s="8">
-        <v>0</v>
-      </c>
-      <c r="X62" s="8">
-        <v>0</v>
-      </c>
-      <c r="Y62" s="8">
-        <v>0</v>
-      </c>
-      <c r="Z62" s="8">
-        <v>0</v>
-      </c>
-      <c r="AA62" s="8">
-        <v>0</v>
-      </c>
-      <c r="AB62" s="8">
-        <v>0</v>
-      </c>
-      <c r="AC62" s="8">
-        <v>0</v>
-      </c>
-      <c r="AD62" s="8">
-        <v>0</v>
-      </c>
-      <c r="AE62" s="8">
-        <v>0</v>
-      </c>
-      <c r="AF62" s="8">
-        <v>0</v>
-      </c>
-      <c r="AG62" s="8">
-        <v>0</v>
-      </c>
-      <c r="AH62" s="8">
-        <v>0</v>
-      </c>
-      <c r="AI62" s="8">
-        <v>0</v>
-      </c>
-      <c r="AJ62" s="8">
-        <v>0</v>
-      </c>
-      <c r="AK62" s="8">
-        <v>0</v>
-      </c>
-      <c r="AL62" s="8">
-        <v>0</v>
-      </c>
-      <c r="AM62" s="8">
-        <v>0</v>
-      </c>
-      <c r="AN62" s="8">
-        <v>0</v>
-      </c>
-      <c r="AO62" s="8">
-        <v>0</v>
-      </c>
     </row>
     <row r="63" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A63" s="56"/>
+      <c r="A63" s="59"/>
       <c r="B63" s="17" t="s">
         <v>50</v>
       </c>
@@ -18340,7 +18340,7 @@
       </c>
     </row>
     <row r="64" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A64" s="56"/>
+      <c r="A64" s="59"/>
       <c r="B64" s="17" t="s">
         <v>51</v>
       </c>
@@ -18399,71 +18399,71 @@
         <v>0</v>
       </c>
       <c r="U64" s="8">
+        <v>0</v>
+      </c>
+      <c r="V64" s="8">
+        <v>0</v>
+      </c>
+      <c r="W64" s="8">
+        <v>0</v>
+      </c>
+      <c r="X64" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y64" s="8">
+        <v>0</v>
+      </c>
+      <c r="Z64" s="8">
+        <v>0</v>
+      </c>
+      <c r="AA64" s="8">
+        <v>0</v>
+      </c>
+      <c r="AB64" s="8">
+        <v>0</v>
+      </c>
+      <c r="AC64" s="8">
+        <v>0</v>
+      </c>
+      <c r="AD64" s="8">
+        <v>0</v>
+      </c>
+      <c r="AE64" s="8">
+        <v>0</v>
+      </c>
+      <c r="AF64" s="8">
+        <v>0</v>
+      </c>
+      <c r="AG64" s="8">
+        <v>0</v>
+      </c>
+      <c r="AH64" s="8">
+        <v>0</v>
+      </c>
+      <c r="AI64" s="8">
+        <v>0</v>
+      </c>
+      <c r="AJ64" s="8">
+        <v>0</v>
+      </c>
+      <c r="AK64" s="8">
+        <v>0</v>
+      </c>
+      <c r="AL64" s="8">
+        <v>0</v>
+      </c>
+      <c r="AM64" s="8">
+        <v>0</v>
+      </c>
+      <c r="AN64" s="8">
+        <v>0</v>
+      </c>
+      <c r="AO64" s="8">
         <v>0.45</v>
       </c>
-      <c r="V64" s="8">
-        <v>0</v>
-      </c>
-      <c r="W64" s="8">
-        <v>0</v>
-      </c>
-      <c r="X64" s="8">
-        <v>0</v>
-      </c>
-      <c r="Y64" s="8">
-        <v>0</v>
-      </c>
-      <c r="Z64" s="8">
-        <v>0</v>
-      </c>
-      <c r="AA64" s="8">
-        <v>0</v>
-      </c>
-      <c r="AB64" s="8">
-        <v>0</v>
-      </c>
-      <c r="AC64" s="8">
-        <v>0</v>
-      </c>
-      <c r="AD64" s="8">
-        <v>0</v>
-      </c>
-      <c r="AE64" s="8">
-        <v>0</v>
-      </c>
-      <c r="AF64" s="8">
-        <v>0</v>
-      </c>
-      <c r="AG64" s="8">
-        <v>0</v>
-      </c>
-      <c r="AH64" s="8">
-        <v>0</v>
-      </c>
-      <c r="AI64" s="8">
-        <v>0</v>
-      </c>
-      <c r="AJ64" s="8">
-        <v>0</v>
-      </c>
-      <c r="AK64" s="8">
-        <v>0</v>
-      </c>
-      <c r="AL64" s="8">
-        <v>0</v>
-      </c>
-      <c r="AM64" s="8">
-        <v>0</v>
-      </c>
-      <c r="AN64" s="8">
-        <v>0</v>
-      </c>
-      <c r="AO64" s="8">
-        <v>0</v>
-      </c>
     </row>
     <row r="65" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A65" s="56"/>
+      <c r="A65" s="59"/>
       <c r="B65" s="17" t="s">
         <v>52</v>
       </c>
@@ -18522,71 +18522,71 @@
         <v>0</v>
       </c>
       <c r="U65" s="8">
+        <v>0</v>
+      </c>
+      <c r="V65" s="8">
+        <v>0</v>
+      </c>
+      <c r="W65" s="8">
+        <v>0</v>
+      </c>
+      <c r="X65" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y65" s="8">
+        <v>0</v>
+      </c>
+      <c r="Z65" s="8">
+        <v>0</v>
+      </c>
+      <c r="AA65" s="8">
+        <v>0</v>
+      </c>
+      <c r="AB65" s="8">
+        <v>0</v>
+      </c>
+      <c r="AC65" s="8">
+        <v>0</v>
+      </c>
+      <c r="AD65" s="8">
+        <v>0</v>
+      </c>
+      <c r="AE65" s="8">
+        <v>0</v>
+      </c>
+      <c r="AF65" s="8">
+        <v>0</v>
+      </c>
+      <c r="AG65" s="8">
+        <v>0</v>
+      </c>
+      <c r="AH65" s="8">
+        <v>0</v>
+      </c>
+      <c r="AI65" s="8">
+        <v>0</v>
+      </c>
+      <c r="AJ65" s="8">
+        <v>0</v>
+      </c>
+      <c r="AK65" s="8">
+        <v>0</v>
+      </c>
+      <c r="AL65" s="8">
+        <v>0</v>
+      </c>
+      <c r="AM65" s="8">
+        <v>0</v>
+      </c>
+      <c r="AN65" s="8">
+        <v>0</v>
+      </c>
+      <c r="AO65" s="8">
         <v>0.35</v>
       </c>
-      <c r="V65" s="8">
-        <v>0</v>
-      </c>
-      <c r="W65" s="8">
-        <v>0</v>
-      </c>
-      <c r="X65" s="8">
-        <v>0</v>
-      </c>
-      <c r="Y65" s="8">
-        <v>0</v>
-      </c>
-      <c r="Z65" s="8">
-        <v>0</v>
-      </c>
-      <c r="AA65" s="8">
-        <v>0</v>
-      </c>
-      <c r="AB65" s="8">
-        <v>0</v>
-      </c>
-      <c r="AC65" s="8">
-        <v>0</v>
-      </c>
-      <c r="AD65" s="8">
-        <v>0</v>
-      </c>
-      <c r="AE65" s="8">
-        <v>0</v>
-      </c>
-      <c r="AF65" s="8">
-        <v>0</v>
-      </c>
-      <c r="AG65" s="8">
-        <v>0</v>
-      </c>
-      <c r="AH65" s="8">
-        <v>0</v>
-      </c>
-      <c r="AI65" s="8">
-        <v>0</v>
-      </c>
-      <c r="AJ65" s="8">
-        <v>0</v>
-      </c>
-      <c r="AK65" s="8">
-        <v>0</v>
-      </c>
-      <c r="AL65" s="8">
-        <v>0</v>
-      </c>
-      <c r="AM65" s="8">
-        <v>0</v>
-      </c>
-      <c r="AN65" s="8">
-        <v>0</v>
-      </c>
-      <c r="AO65" s="8">
-        <v>0</v>
-      </c>
     </row>
     <row r="66" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A66" s="57"/>
+      <c r="A66" s="60"/>
       <c r="B66" s="18" t="s">
         <v>53</v>
       </c>
@@ -18645,71 +18645,71 @@
         <v>0</v>
       </c>
       <c r="U66" s="15">
+        <v>0</v>
+      </c>
+      <c r="V66" s="15">
+        <v>0</v>
+      </c>
+      <c r="W66" s="15">
+        <v>0</v>
+      </c>
+      <c r="X66" s="15">
+        <v>0</v>
+      </c>
+      <c r="Y66" s="15">
+        <v>0</v>
+      </c>
+      <c r="Z66" s="15">
+        <v>0</v>
+      </c>
+      <c r="AA66" s="15">
+        <v>0</v>
+      </c>
+      <c r="AB66" s="15">
+        <v>0</v>
+      </c>
+      <c r="AC66" s="15">
+        <v>0</v>
+      </c>
+      <c r="AD66" s="15">
+        <v>0</v>
+      </c>
+      <c r="AE66" s="15">
+        <v>0</v>
+      </c>
+      <c r="AF66" s="15">
+        <v>0</v>
+      </c>
+      <c r="AG66" s="15">
+        <v>0</v>
+      </c>
+      <c r="AH66" s="15">
+        <v>0</v>
+      </c>
+      <c r="AI66" s="15">
+        <v>0</v>
+      </c>
+      <c r="AJ66" s="15">
+        <v>0</v>
+      </c>
+      <c r="AK66" s="15">
+        <v>0</v>
+      </c>
+      <c r="AL66" s="15">
+        <v>0</v>
+      </c>
+      <c r="AM66" s="15">
+        <v>0</v>
+      </c>
+      <c r="AN66" s="15">
+        <v>0</v>
+      </c>
+      <c r="AO66" s="15">
         <v>0.37</v>
       </c>
-      <c r="V66" s="15">
-        <v>0</v>
-      </c>
-      <c r="W66" s="15">
-        <v>0</v>
-      </c>
-      <c r="X66" s="15">
-        <v>0</v>
-      </c>
-      <c r="Y66" s="15">
-        <v>0</v>
-      </c>
-      <c r="Z66" s="15">
-        <v>0</v>
-      </c>
-      <c r="AA66" s="15">
-        <v>0</v>
-      </c>
-      <c r="AB66" s="15">
-        <v>0</v>
-      </c>
-      <c r="AC66" s="15">
-        <v>0</v>
-      </c>
-      <c r="AD66" s="15">
-        <v>0</v>
-      </c>
-      <c r="AE66" s="15">
-        <v>0</v>
-      </c>
-      <c r="AF66" s="15">
-        <v>0</v>
-      </c>
-      <c r="AG66" s="15">
-        <v>0</v>
-      </c>
-      <c r="AH66" s="15">
-        <v>0</v>
-      </c>
-      <c r="AI66" s="15">
-        <v>0</v>
-      </c>
-      <c r="AJ66" s="15">
-        <v>0</v>
-      </c>
-      <c r="AK66" s="15">
-        <v>0</v>
-      </c>
-      <c r="AL66" s="15">
-        <v>0</v>
-      </c>
-      <c r="AM66" s="15">
-        <v>0</v>
-      </c>
-      <c r="AN66" s="15">
-        <v>0</v>
-      </c>
-      <c r="AO66" s="15">
-        <v>0</v>
-      </c>
     </row>
     <row r="67" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A67" s="55" t="s">
+      <c r="A67" s="58" t="s">
         <v>54</v>
       </c>
       <c r="B67" s="11" t="s">
@@ -18834,7 +18834,7 @@
       </c>
     </row>
     <row r="68" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A68" s="56"/>
+      <c r="A68" s="59"/>
       <c r="B68" s="17" t="s">
         <v>55</v>
       </c>
@@ -18957,7 +18957,7 @@
       </c>
     </row>
     <row r="69" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A69" s="57"/>
+      <c r="A69" s="60"/>
       <c r="B69" s="18" t="s">
         <v>56</v>
       </c>
@@ -19113,7 +19113,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5A29F17-D94C-4A81-8A6D-42D62B17E419}">
   <dimension ref="A1:AO41"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A32" sqref="A32:Y33"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add separate power flow module and export node-level load data
</commit_message>
<xml_diff>
--- a/Input Data - Resources 1.xlsx
+++ b/Input Data - Resources 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hugo.serrano\PycharmProjects1\CRETE_VALLEY_T.4.3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDE619BC-2635-4EB3-A886-B0FD24037D39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD41B1B7-9192-4F91-A70D-8BF3E9599FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="907" activeTab="3" xr2:uid="{A643D732-D500-40EC-92C3-BB1380872BE9}"/>
   </bookViews>
@@ -932,8 +932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{293146E6-8E2D-4ADC-82E7-CE7DA50FFBD7}">
   <dimension ref="A2:Z43"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18:Z18"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12:Z12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2181,76 +2181,76 @@
         <v>16</v>
       </c>
       <c r="C18" s="54">
-        <v>77.081639600000003</v>
+        <v>0</v>
       </c>
       <c r="D18" s="54">
-        <v>76.205639599999998</v>
+        <v>0</v>
       </c>
       <c r="E18" s="54">
-        <v>77.573806099999999</v>
+        <v>0</v>
       </c>
       <c r="F18" s="54">
-        <v>75.894639600000005</v>
+        <v>0</v>
       </c>
       <c r="G18" s="54">
-        <v>76.521139499999904</v>
+        <v>0</v>
       </c>
       <c r="H18" s="54">
-        <v>78.041639599999996</v>
+        <v>0</v>
       </c>
       <c r="I18" s="54">
-        <v>138.90155632000003</v>
+        <v>0</v>
       </c>
       <c r="J18" s="54">
-        <v>107.0398029</v>
+        <v>0</v>
       </c>
       <c r="K18" s="54">
-        <v>141.36430200000001</v>
+        <v>0</v>
       </c>
       <c r="L18" s="54">
-        <v>174.7566344</v>
+        <v>0</v>
       </c>
       <c r="M18" s="54">
-        <v>176.8601353</v>
+        <v>0</v>
       </c>
       <c r="N18" s="54">
-        <v>176.50713210000001</v>
+        <v>0</v>
       </c>
       <c r="O18" s="54">
-        <v>176.68196620000001</v>
+        <v>0</v>
       </c>
       <c r="P18" s="54">
-        <v>177.60013069999999</v>
+        <v>0</v>
       </c>
       <c r="Q18" s="54">
-        <v>173.07829939999999</v>
+        <v>0</v>
       </c>
       <c r="R18" s="54">
-        <v>172.9864657</v>
+        <v>0</v>
       </c>
       <c r="S18" s="54">
-        <v>171.86096659999899</v>
+        <v>0</v>
       </c>
       <c r="T18" s="54">
-        <v>254.45574360000003</v>
+        <v>0</v>
       </c>
       <c r="U18" s="54">
-        <v>213.27413530000001</v>
+        <v>0</v>
       </c>
       <c r="V18" s="54">
-        <v>201.42347029999999</v>
+        <v>0</v>
       </c>
       <c r="W18" s="54">
-        <v>193.4893036</v>
+        <v>0</v>
       </c>
       <c r="X18" s="54">
-        <v>90.646970199999998</v>
+        <v>0</v>
       </c>
       <c r="Y18" s="54">
-        <v>86.497136900000001</v>
+        <v>0</v>
       </c>
       <c r="Z18" s="54">
-        <v>84.372804500000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:26" x14ac:dyDescent="0.35">
@@ -2258,76 +2258,76 @@
         <v>17</v>
       </c>
       <c r="C19" s="54">
-        <v>77.081639600000003</v>
+        <v>0</v>
       </c>
       <c r="D19" s="54">
-        <v>76.205639599999998</v>
+        <v>0</v>
       </c>
       <c r="E19" s="54">
-        <v>77.573806099999999</v>
+        <v>0</v>
       </c>
       <c r="F19" s="54">
-        <v>75.894639600000005</v>
+        <v>0</v>
       </c>
       <c r="G19" s="54">
-        <v>76.521139499999904</v>
+        <v>0</v>
       </c>
       <c r="H19" s="54">
-        <v>78.041639599999996</v>
+        <v>0</v>
       </c>
       <c r="I19" s="54">
-        <v>138.90155632000003</v>
+        <v>0</v>
       </c>
       <c r="J19" s="54">
-        <v>107.0398029</v>
+        <v>0</v>
       </c>
       <c r="K19" s="54">
-        <v>141.36430200000001</v>
+        <v>0</v>
       </c>
       <c r="L19" s="54">
-        <v>174.7566344</v>
+        <v>0</v>
       </c>
       <c r="M19" s="54">
-        <v>176.8601353</v>
+        <v>0</v>
       </c>
       <c r="N19" s="54">
-        <v>176.50713210000001</v>
+        <v>0</v>
       </c>
       <c r="O19" s="54">
-        <v>176.68196620000001</v>
+        <v>0</v>
       </c>
       <c r="P19" s="54">
-        <v>177.60013069999999</v>
+        <v>0</v>
       </c>
       <c r="Q19" s="54">
-        <v>173.07829939999999</v>
+        <v>0</v>
       </c>
       <c r="R19" s="54">
-        <v>172.9864657</v>
+        <v>0</v>
       </c>
       <c r="S19" s="54">
-        <v>171.86096659999899</v>
+        <v>0</v>
       </c>
       <c r="T19" s="54">
-        <v>254.45574360000003</v>
+        <v>0</v>
       </c>
       <c r="U19" s="54">
-        <v>213.27413530000001</v>
+        <v>0</v>
       </c>
       <c r="V19" s="54">
-        <v>201.42347029999999</v>
+        <v>0</v>
       </c>
       <c r="W19" s="54">
-        <v>193.4893036</v>
+        <v>0</v>
       </c>
       <c r="X19" s="54">
-        <v>90.646970199999998</v>
+        <v>0</v>
       </c>
       <c r="Y19" s="54">
-        <v>86.497136900000001</v>
+        <v>0</v>
       </c>
       <c r="Z19" s="54">
-        <v>84.372804500000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:26" x14ac:dyDescent="0.35">
@@ -3567,76 +3567,76 @@
         <v>34</v>
       </c>
       <c r="C36" s="54">
-        <v>77.081639600000003</v>
+        <v>0</v>
       </c>
       <c r="D36" s="54">
-        <v>76.205639599999998</v>
+        <v>0</v>
       </c>
       <c r="E36" s="54">
-        <v>77.573806099999999</v>
+        <v>0</v>
       </c>
       <c r="F36" s="54">
-        <v>75.894639600000005</v>
+        <v>0</v>
       </c>
       <c r="G36" s="54">
-        <v>76.521139499999904</v>
+        <v>0</v>
       </c>
       <c r="H36" s="54">
-        <v>78.041639599999996</v>
+        <v>0</v>
       </c>
       <c r="I36" s="54">
-        <v>138.90155632000003</v>
+        <v>0</v>
       </c>
       <c r="J36" s="54">
-        <v>107.0398029</v>
+        <v>0</v>
       </c>
       <c r="K36" s="54">
-        <v>141.36430200000001</v>
+        <v>0</v>
       </c>
       <c r="L36" s="54">
-        <v>174.7566344</v>
+        <v>0</v>
       </c>
       <c r="M36" s="54">
-        <v>176.8601353</v>
+        <v>0</v>
       </c>
       <c r="N36" s="54">
-        <v>176.50713210000001</v>
+        <v>0</v>
       </c>
       <c r="O36" s="54">
-        <v>176.68196620000001</v>
+        <v>0</v>
       </c>
       <c r="P36" s="54">
-        <v>177.60013069999999</v>
+        <v>0</v>
       </c>
       <c r="Q36" s="54">
-        <v>173.07829939999999</v>
+        <v>0</v>
       </c>
       <c r="R36" s="54">
-        <v>172.9864657</v>
+        <v>0</v>
       </c>
       <c r="S36" s="54">
-        <v>171.86096659999899</v>
+        <v>0</v>
       </c>
       <c r="T36" s="54">
-        <v>254.45574360000003</v>
+        <v>0</v>
       </c>
       <c r="U36" s="54">
-        <v>213.27413530000001</v>
+        <v>0</v>
       </c>
       <c r="V36" s="54">
-        <v>201.42347029999999</v>
+        <v>0</v>
       </c>
       <c r="W36" s="54">
-        <v>193.4893036</v>
+        <v>0</v>
       </c>
       <c r="X36" s="54">
-        <v>90.646970199999998</v>
+        <v>0</v>
       </c>
       <c r="Y36" s="54">
-        <v>86.497136900000001</v>
+        <v>0</v>
       </c>
       <c r="Z36" s="54">
-        <v>84.372804500000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="2:26" x14ac:dyDescent="0.35">
@@ -3875,76 +3875,76 @@
         <v>38</v>
       </c>
       <c r="C40" s="54">
-        <v>77.081639600000003</v>
+        <v>0</v>
       </c>
       <c r="D40" s="54">
-        <v>76.205639599999998</v>
+        <v>0</v>
       </c>
       <c r="E40" s="54">
-        <v>77.573806099999999</v>
+        <v>0</v>
       </c>
       <c r="F40" s="54">
-        <v>75.894639600000005</v>
+        <v>0</v>
       </c>
       <c r="G40" s="54">
-        <v>76.521139499999904</v>
+        <v>0</v>
       </c>
       <c r="H40" s="54">
-        <v>78.041639599999996</v>
+        <v>0</v>
       </c>
       <c r="I40" s="54">
-        <v>138.90155632000003</v>
+        <v>0</v>
       </c>
       <c r="J40" s="54">
-        <v>107.0398029</v>
+        <v>0</v>
       </c>
       <c r="K40" s="54">
-        <v>141.36430200000001</v>
+        <v>0</v>
       </c>
       <c r="L40" s="54">
-        <v>174.7566344</v>
+        <v>0</v>
       </c>
       <c r="M40" s="54">
-        <v>176.8601353</v>
+        <v>0</v>
       </c>
       <c r="N40" s="54">
-        <v>176.50713210000001</v>
+        <v>0</v>
       </c>
       <c r="O40" s="54">
-        <v>176.68196620000001</v>
+        <v>0</v>
       </c>
       <c r="P40" s="54">
-        <v>177.60013069999999</v>
+        <v>0</v>
       </c>
       <c r="Q40" s="54">
-        <v>173.07829939999999</v>
+        <v>0</v>
       </c>
       <c r="R40" s="54">
-        <v>172.9864657</v>
+        <v>0</v>
       </c>
       <c r="S40" s="54">
-        <v>171.86096659999899</v>
+        <v>0</v>
       </c>
       <c r="T40" s="54">
-        <v>254.45574360000003</v>
+        <v>0</v>
       </c>
       <c r="U40" s="54">
-        <v>213.27413530000001</v>
+        <v>0</v>
       </c>
       <c r="V40" s="54">
-        <v>201.42347029999999</v>
+        <v>0</v>
       </c>
       <c r="W40" s="54">
-        <v>193.4893036</v>
+        <v>0</v>
       </c>
       <c r="X40" s="54">
-        <v>90.646970199999998</v>
+        <v>0</v>
       </c>
       <c r="Y40" s="54">
-        <v>86.497136900000001</v>
+        <v>0</v>
       </c>
       <c r="Z40" s="54">
-        <v>84.372804500000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="2:26" x14ac:dyDescent="0.35">
@@ -10285,7 +10285,7 @@
   <dimension ref="A2:IE70"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AH61" sqref="AH61:AH66"/>
+      <selection activeCell="L3" sqref="L3:L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13162,16 +13162,16 @@
         <v>1</v>
       </c>
       <c r="K25" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L25" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M25" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N25" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O25" s="13">
         <v>0</v>
@@ -13183,10 +13183,10 @@
         <v>0</v>
       </c>
       <c r="R25" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S25" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T25" s="13">
         <v>0</v>
@@ -13198,7 +13198,7 @@
         <v>0</v>
       </c>
       <c r="W25" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X25" s="13">
         <v>0</v>
@@ -13207,7 +13207,7 @@
         <v>0</v>
       </c>
       <c r="Z25" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA25" s="13">
         <v>0</v>
@@ -13285,16 +13285,16 @@
         <v>10</v>
       </c>
       <c r="K26" s="15">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="L26" s="15">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="M26" s="15">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="N26" s="15">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="O26" s="15">
         <v>0</v>
@@ -13306,10 +13306,10 @@
         <v>0</v>
       </c>
       <c r="R26" s="15">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="S26" s="15">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="T26" s="15">
         <v>0</v>
@@ -13321,7 +13321,7 @@
         <v>0</v>
       </c>
       <c r="W26" s="15">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="X26" s="15">
         <v>0</v>
@@ -13330,7 +13330,7 @@
         <v>0</v>
       </c>
       <c r="Z26" s="15">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AA26" s="15">
         <v>0</v>
@@ -16169,7 +16169,7 @@
         <v>0</v>
       </c>
       <c r="Q46" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R46" s="13">
         <v>0</v>
@@ -16187,7 +16187,7 @@
         <v>0</v>
       </c>
       <c r="W46" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X46" s="13">
         <v>0</v>
@@ -16214,7 +16214,7 @@
         <v>0</v>
       </c>
       <c r="AF46" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG46" s="13">
         <v>0</v>
@@ -16292,7 +16292,7 @@
         <v>0</v>
       </c>
       <c r="Q47" s="8">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="R47" s="8">
         <v>0</v>
@@ -16310,7 +16310,7 @@
         <v>0</v>
       </c>
       <c r="W47" s="8">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="X47" s="8">
         <v>0</v>
@@ -16337,7 +16337,7 @@
         <v>0</v>
       </c>
       <c r="AF47" s="8">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AG47" s="8">
         <v>0</v>
@@ -16415,7 +16415,7 @@
         <v>0</v>
       </c>
       <c r="Q48" s="8">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="R48" s="8">
         <v>0</v>
@@ -16433,7 +16433,7 @@
         <v>0</v>
       </c>
       <c r="W48" s="8">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="X48" s="8">
         <v>0</v>
@@ -16460,7 +16460,7 @@
         <v>0</v>
       </c>
       <c r="AF48" s="8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AG48" s="8">
         <v>0</v>
@@ -16538,7 +16538,7 @@
         <v>0</v>
       </c>
       <c r="Q49" s="8">
-        <v>0</v>
+        <v>0.85</v>
       </c>
       <c r="R49" s="8">
         <v>0</v>
@@ -16556,7 +16556,7 @@
         <v>0</v>
       </c>
       <c r="W49" s="8">
-        <v>0</v>
+        <v>0.85</v>
       </c>
       <c r="X49" s="8">
         <v>0</v>
@@ -16583,7 +16583,7 @@
         <v>0</v>
       </c>
       <c r="AF49" s="8">
-        <v>0</v>
+        <v>0.85</v>
       </c>
       <c r="AG49" s="8">
         <v>0</v>
@@ -16661,7 +16661,7 @@
         <v>0</v>
       </c>
       <c r="Q50" s="8">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="R50" s="8">
         <v>0</v>
@@ -16679,7 +16679,7 @@
         <v>0</v>
       </c>
       <c r="W50" s="8">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="X50" s="8">
         <v>0</v>
@@ -16706,7 +16706,7 @@
         <v>0</v>
       </c>
       <c r="AF50" s="8">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="AG50" s="8">
         <v>0</v>
@@ -16784,7 +16784,7 @@
         <v>0</v>
       </c>
       <c r="Q51" s="15">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="R51" s="15">
         <v>0</v>
@@ -16802,7 +16802,7 @@
         <v>0</v>
       </c>
       <c r="W51" s="15">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="X51" s="15">
         <v>0</v>
@@ -16829,7 +16829,7 @@
         <v>0</v>
       </c>
       <c r="AF51" s="15">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="AG51" s="15">
         <v>0</v>
@@ -18009,7 +18009,7 @@
         <v>0</v>
       </c>
       <c r="N61" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O61" s="8">
         <v>0</v>
@@ -18030,7 +18030,7 @@
         <v>0</v>
       </c>
       <c r="U61" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V61" s="8">
         <v>0</v>
@@ -18069,7 +18069,7 @@
         <v>0</v>
       </c>
       <c r="AH61" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI61" s="8">
         <v>0</v>
@@ -18132,7 +18132,7 @@
         <v>0</v>
       </c>
       <c r="N62" s="8">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="O62" s="8">
         <v>0</v>
@@ -18153,7 +18153,7 @@
         <v>0</v>
       </c>
       <c r="U62" s="8">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="V62" s="8">
         <v>0</v>
@@ -18192,7 +18192,7 @@
         <v>0</v>
       </c>
       <c r="AH62" s="8">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="AI62" s="8">
         <v>0</v>
@@ -18378,7 +18378,7 @@
         <v>0</v>
       </c>
       <c r="N64" s="8">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="O64" s="8">
         <v>0</v>
@@ -18399,7 +18399,7 @@
         <v>0</v>
       </c>
       <c r="U64" s="8">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="V64" s="8">
         <v>0</v>
@@ -18438,7 +18438,7 @@
         <v>0</v>
       </c>
       <c r="AH64" s="8">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="AI64" s="8">
         <v>0</v>
@@ -18501,7 +18501,7 @@
         <v>0</v>
       </c>
       <c r="N65" s="8">
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="O65" s="8">
         <v>0</v>
@@ -18522,7 +18522,7 @@
         <v>0</v>
       </c>
       <c r="U65" s="8">
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="V65" s="8">
         <v>0</v>
@@ -18561,7 +18561,7 @@
         <v>0</v>
       </c>
       <c r="AH65" s="8">
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="AI65" s="8">
         <v>0</v>
@@ -18624,7 +18624,7 @@
         <v>0</v>
       </c>
       <c r="N66" s="15">
-        <v>0</v>
+        <v>0.37</v>
       </c>
       <c r="O66" s="15">
         <v>0</v>
@@ -18645,7 +18645,7 @@
         <v>0</v>
       </c>
       <c r="U66" s="15">
-        <v>0</v>
+        <v>0.37</v>
       </c>
       <c r="V66" s="15">
         <v>0</v>
@@ -18684,7 +18684,7 @@
         <v>0</v>
       </c>
       <c r="AH66" s="15">
-        <v>0</v>
+        <v>0.37</v>
       </c>
       <c r="AI66" s="15">
         <v>0</v>
@@ -32041,21 +32041,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006EB96E01841F534A9C78DC9E98988F27" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e9cd0784f49f37c1a173dce4a7ba0add">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="768b940a-12b3-4bec-8bc4-e76c6f92f4e8" xmlns:ns4="825cedbc-969e-4d8d-87a7-78044fba72ff" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d0f00a3aa6de0fd555e3fea5893c31c9" ns3:_="" ns4:_="">
     <xsd:import namespace="768b940a-12b3-4bec-8bc4-e76c6f92f4e8"/>
@@ -32266,32 +32251,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47108D9C-9F22-4BF8-A049-F9C9D73243DC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="825cedbc-969e-4d8d-87a7-78044fba72ff"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="768b940a-12b3-4bec-8bc4-e76c6f92f4e8"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00860459-9AB3-404C-9E09-2F98C31A67E6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD02C117-BEF2-48D5-9623-486F204F6E0B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -32308,4 +32283,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00860459-9AB3-404C-9E09-2F98C31A67E6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47108D9C-9F22-4BF8-A049-F9C9D73243DC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="825cedbc-969e-4d8d-87a7-78044fba72ff"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="768b940a-12b3-4bec-8bc4-e76c6f92f4e8"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>